<commit_message>
Update clinical data list ADNI
Former-commit-id: 9b7b1dbe84452c2665ee3ced61d6c6a76e7d99ae
</commit_message>
<xml_diff>
--- a/clinica/iotools/data/clinical_specifications_adni.xlsx
+++ b/clinica/iotools/data/clinical_specifications_adni.xlsx
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="271">
   <si>
     <t>Field</t>
   </si>
@@ -835,6 +835,36 @@
   </si>
   <si>
     <t>DIGITSCOR</t>
+  </si>
+  <si>
+    <t>Fusiform</t>
+  </si>
+  <si>
+    <t>MidTemp</t>
+  </si>
+  <si>
+    <t>adni_fusiform_vol</t>
+  </si>
+  <si>
+    <t>adni_midtemp_vol</t>
+  </si>
+  <si>
+    <t>adni_abeta</t>
+  </si>
+  <si>
+    <t>adni_tau</t>
+  </si>
+  <si>
+    <t>adni_ptau</t>
+  </si>
+  <si>
+    <t>ABETA</t>
+  </si>
+  <si>
+    <t>TAU</t>
+  </si>
+  <si>
+    <t>PTAU</t>
   </si>
 </sst>
 </file>
@@ -3230,6 +3260,118 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1498600</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="40" name="AutoShape 1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="12839700" cy="12700000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="r" b="b"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1498600</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="41" name="AutoShape 1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="12839700" cy="12700000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="r" b="b"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -8964,10 +9106,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F62"/>
+  <dimension ref="A1:F68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="C67" sqref="C67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -10056,6 +10198,76 @@
         <v>206</v>
       </c>
       <c r="F62" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B64" s="15" t="s">
+        <v>263</v>
+      </c>
+      <c r="C64" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="E64" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="F64" s="15" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="65" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B65" s="15" t="s">
+        <v>264</v>
+      </c>
+      <c r="C65" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="E65" s="15" t="s">
+        <v>262</v>
+      </c>
+      <c r="F65" s="15" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="66" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B66" s="15" t="s">
+        <v>265</v>
+      </c>
+      <c r="C66" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="E66" s="15" t="s">
+        <v>268</v>
+      </c>
+      <c r="F66" s="15" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="67" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B67" s="15" t="s">
+        <v>266</v>
+      </c>
+      <c r="C67" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="E67" s="15" t="s">
+        <v>269</v>
+      </c>
+      <c r="F67" s="15" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="68" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B68" s="15" t="s">
+        <v>267</v>
+      </c>
+      <c r="C68" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="E68" s="15" t="s">
+        <v>270</v>
+      </c>
+      <c r="F68" s="15" t="s">
         <v>95</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add age at baseline
</commit_message>
<xml_diff>
--- a/clinica/iotools/data/clinical_specifications_adni.xlsx
+++ b/clinica/iotools/data/clinical_specifications_adni.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16180" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2400" windowWidth="28800" windowHeight="16180" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="participant.tsv" sheetId="1" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2193" uniqueCount="1346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2195" uniqueCount="1346">
   <si>
     <t>Field</t>
   </si>
@@ -4419,7 +4419,7 @@
         <xdr:cNvPr id="1025" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000001040000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4476,7 +4476,7 @@
         <xdr:cNvPr id="2" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4533,7 +4533,7 @@
         <xdr:cNvPr id="3" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4590,7 +4590,7 @@
         <xdr:cNvPr id="4" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4647,7 +4647,7 @@
         <xdr:cNvPr id="5" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000005000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4704,7 +4704,7 @@
         <xdr:cNvPr id="6" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000006000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4761,7 +4761,7 @@
         <xdr:cNvPr id="7" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000007000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4818,7 +4818,7 @@
         <xdr:cNvPr id="8" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000008000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4875,7 +4875,7 @@
         <xdr:cNvPr id="9" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000009000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4932,7 +4932,7 @@
         <xdr:cNvPr id="10" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000A000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4989,7 +4989,7 @@
         <xdr:cNvPr id="11" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000B000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5046,7 +5046,7 @@
         <xdr:cNvPr id="12" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000C000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5103,7 +5103,7 @@
         <xdr:cNvPr id="13" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000D000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5160,7 +5160,7 @@
         <xdr:cNvPr id="14" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000E000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5217,7 +5217,7 @@
         <xdr:cNvPr id="15" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000F000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5274,7 +5274,7 @@
         <xdr:cNvPr id="16" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000010000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000010000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5331,7 +5331,7 @@
         <xdr:cNvPr id="17" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000011000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000011000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5388,7 +5388,7 @@
         <xdr:cNvPr id="18" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000012000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000012000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5445,7 +5445,7 @@
         <xdr:cNvPr id="19" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000013000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000013000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5502,7 +5502,7 @@
         <xdr:cNvPr id="20" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000014000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000014000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5559,7 +5559,7 @@
         <xdr:cNvPr id="21" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000015000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000015000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5616,7 +5616,7 @@
         <xdr:cNvPr id="22" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000016000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000016000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5673,7 +5673,7 @@
         <xdr:cNvPr id="23" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000017000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000017000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5730,7 +5730,7 @@
         <xdr:cNvPr id="24" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000018000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000018000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5787,7 +5787,7 @@
         <xdr:cNvPr id="25" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000019000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000019000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5844,7 +5844,7 @@
         <xdr:cNvPr id="26" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00001A000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5901,7 +5901,7 @@
         <xdr:cNvPr id="27" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00001B000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5958,7 +5958,7 @@
         <xdr:cNvPr id="28" name="AutoShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00001C000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6020,7 +6020,7 @@
         <xdr:cNvPr id="29" name="AutoShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00001D000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6082,7 +6082,7 @@
         <xdr:cNvPr id="30" name="AutoShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00001E000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6144,7 +6144,7 @@
         <xdr:cNvPr id="31" name="AutoShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00001F000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6206,7 +6206,7 @@
         <xdr:cNvPr id="32" name="AutoShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000020000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000020000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6268,7 +6268,7 @@
         <xdr:cNvPr id="33" name="AutoShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000021000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000021000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6330,7 +6330,7 @@
         <xdr:cNvPr id="34" name="AutoShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000022000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000022000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6392,7 +6392,7 @@
         <xdr:cNvPr id="35" name="AutoShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000023000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000023000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6454,7 +6454,7 @@
         <xdr:cNvPr id="36" name="AutoShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000024000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000024000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6516,7 +6516,7 @@
         <xdr:cNvPr id="37" name="AutoShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000025000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000025000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6578,7 +6578,7 @@
         <xdr:cNvPr id="38" name="AutoShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000026000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000026000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6640,7 +6640,7 @@
         <xdr:cNvPr id="39" name="AutoShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000027000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000027000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6702,7 +6702,7 @@
         <xdr:cNvPr id="40" name="AutoShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000028000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000028000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6764,7 +6764,7 @@
         <xdr:cNvPr id="41" name="AutoShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000029000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000029000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6826,7 +6826,7 @@
         <xdr:cNvPr id="42" name="AutoShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00002A000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6880,7 +6880,7 @@
         <xdr:cNvPr id="43" name="AutoShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6C4D69D0-1097-4046-8882-5C40E94B04AA}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C4D69D0-1097-4046-8882-5C40E94B04AA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6940,6 +6940,62 @@
         <a:xfrm>
           <a:off x="0" y="0"/>
           <a:ext cx="16548100" cy="12700000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1498600</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="45" name="AutoShape 1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="15671800" cy="12700000"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -7240,8 +7296,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -7480,6 +7536,12 @@
       <c r="D11" s="6" t="s">
         <v>69</v>
       </c>
+      <c r="E11" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>85</v>
+      </c>
       <c r="I11" s="12"/>
       <c r="J11" s="12"/>
       <c r="K11" s="12"/>
@@ -7861,7 +7923,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F656"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add ADNI composite scores to sub-xxxx-sessions.tsv file
</commit_message>
<xml_diff>
--- a/clinica/iotools/data/clinical_specifications_adni.xlsx
+++ b/clinica/iotools/data/clinical_specifications_adni.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elina.thibeausutre/Documents/code/clinica/clinica/iotools/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/omar.elrifai/workspace/clinica_fork/clinica/iotools/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{680EFAB6-B34D-DD45-B2F0-7A0C4667F4EB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBD2960E-D5E6-EF42-9615-23C69DB6C8AD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="400" yWindow="1140" windowWidth="28800" windowHeight="16280" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1140" windowWidth="28800" windowHeight="16280" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="participant.tsv" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3530" uniqueCount="2370">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3546" uniqueCount="2381">
   <si>
     <t>Field</t>
   </si>
@@ -7155,6 +7155,39 @@
   </si>
   <si>
     <t>1.0 or 1.5 or 3.0 or 7.0</t>
+  </si>
+  <si>
+    <t>Composite score for memory</t>
+  </si>
+  <si>
+    <t>Composite score for executive functioning</t>
+  </si>
+  <si>
+    <t>Composite score for language</t>
+  </si>
+  <si>
+    <t>Composite score for visuospatial functioning</t>
+  </si>
+  <si>
+    <t>ADNI_LAN</t>
+  </si>
+  <si>
+    <t>ADNI_VS</t>
+  </si>
+  <si>
+    <t>UWNPSYCHSUM_03_26_20.csv</t>
+  </si>
+  <si>
+    <t>comp_mem</t>
+  </si>
+  <si>
+    <t>comp_ef</t>
+  </si>
+  <si>
+    <t>comp_lang</t>
+  </si>
+  <si>
+    <t>comp_vsf</t>
   </si>
 </sst>
 </file>
@@ -7599,7 +7632,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="55.5" style="14" customWidth="1"/>
+    <col min="1" max="1" width="113.5" style="14" customWidth="1"/>
     <col min="2" max="2" width="18.6640625" style="14" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="35.1640625" style="14" customWidth="1"/>
     <col min="4" max="4" width="17.33203125" style="14" customWidth="1"/>
@@ -8227,16 +8260,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F838"/>
+  <dimension ref="A1:F842"/>
   <sheetViews>
-    <sheetView zoomScale="94" zoomScaleNormal="30" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C449" sqref="C449"/>
+    <sheetView tabSelected="1" zoomScale="94" zoomScaleNormal="30" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A805" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B848" sqref="B848"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="39" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="39" style="1" customWidth="1"/>
+    <col min="1" max="1" width="84" style="1" customWidth="1"/>
     <col min="2" max="16384" width="39" style="1"/>
   </cols>
   <sheetData>
@@ -21700,6 +21733,62 @@
       </c>
       <c r="F838" t="s">
         <v>2354</v>
+      </c>
+    </row>
+    <row r="839" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A839" s="1" t="s">
+        <v>2370</v>
+      </c>
+      <c r="B839" s="1" t="s">
+        <v>2377</v>
+      </c>
+      <c r="E839" s="1" t="s">
+        <v>2353</v>
+      </c>
+      <c r="F839" s="1" t="s">
+        <v>2376</v>
+      </c>
+    </row>
+    <row r="840" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A840" s="1" t="s">
+        <v>2371</v>
+      </c>
+      <c r="B840" s="1" t="s">
+        <v>2378</v>
+      </c>
+      <c r="E840" s="1" t="s">
+        <v>2357</v>
+      </c>
+      <c r="F840" s="1" t="s">
+        <v>2376</v>
+      </c>
+    </row>
+    <row r="841" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A841" s="1" t="s">
+        <v>2372</v>
+      </c>
+      <c r="B841" s="1" t="s">
+        <v>2379</v>
+      </c>
+      <c r="E841" s="1" t="s">
+        <v>2374</v>
+      </c>
+      <c r="F841" s="1" t="s">
+        <v>2376</v>
+      </c>
+    </row>
+    <row r="842" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A842" s="1" t="s">
+        <v>2373</v>
+      </c>
+      <c r="B842" s="1" t="s">
+        <v>2380</v>
+      </c>
+      <c r="E842" s="1" t="s">
+        <v>2375</v>
+      </c>
+      <c r="F842" s="1" t="s">
+        <v>2376</v>
       </c>
     </row>
   </sheetData>
@@ -21712,7 +21801,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
update clinica_specifications_adni.xlsx with SP info
</commit_message>
<xml_diff>
--- a/clinica/iotools/data/clinical_specifications_adni.xlsx
+++ b/clinica/iotools/data/clinical_specifications_adni.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/omar.elrifai/workspace/clinica_fork/clinica/iotools/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBD2960E-D5E6-EF42-9615-23C69DB6C8AD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C84E7CE8-17EA-9C4E-8F01-C9BE6D00AA1E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1140" windowWidth="28800" windowHeight="16280" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3546" uniqueCount="2381">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3546" uniqueCount="2388">
   <si>
     <t>Field</t>
   </si>
@@ -7188,6 +7188,27 @@
   </si>
   <si>
     <t>comp_vsf</t>
+  </si>
+  <si>
+    <t>EcogSPDivatt</t>
+  </si>
+  <si>
+    <t>EcogSPLang</t>
+  </si>
+  <si>
+    <t>EcogSPMem</t>
+  </si>
+  <si>
+    <t>EcogSPOrgan</t>
+  </si>
+  <si>
+    <t>EcogSPPlan</t>
+  </si>
+  <si>
+    <t>EcogSPVisspat</t>
+  </si>
+  <si>
+    <t>EcogSPTotal</t>
   </si>
 </sst>
 </file>
@@ -8262,9 +8283,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F842"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="94" zoomScaleNormal="30" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A805" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B848" sqref="B848"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="94" zoomScaleNormal="30" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A232" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E255" sqref="E255"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="39" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -12361,7 +12382,7 @@
       <c r="C246"/>
       <c r="D246"/>
       <c r="E246" t="s">
-        <v>582</v>
+        <v>2381</v>
       </c>
       <c r="F246" t="s">
         <v>603</v>
@@ -12377,7 +12398,7 @@
       <c r="C247"/>
       <c r="D247"/>
       <c r="E247" t="s">
-        <v>585</v>
+        <v>2382</v>
       </c>
       <c r="F247" t="s">
         <v>603</v>
@@ -12393,7 +12414,7 @@
       <c r="C248"/>
       <c r="D248"/>
       <c r="E248" t="s">
-        <v>588</v>
+        <v>2383</v>
       </c>
       <c r="F248" t="s">
         <v>603</v>
@@ -12409,7 +12430,7 @@
       <c r="C249"/>
       <c r="D249"/>
       <c r="E249" t="s">
-        <v>591</v>
+        <v>2384</v>
       </c>
       <c r="F249" t="s">
         <v>603</v>
@@ -12425,7 +12446,7 @@
       <c r="C250"/>
       <c r="D250"/>
       <c r="E250" t="s">
-        <v>594</v>
+        <v>2385</v>
       </c>
       <c r="F250" t="s">
         <v>603</v>
@@ -12441,7 +12462,7 @@
       <c r="C251"/>
       <c r="D251"/>
       <c r="E251" t="s">
-        <v>597</v>
+        <v>2386</v>
       </c>
       <c r="F251" t="s">
         <v>603</v>
@@ -12457,7 +12478,7 @@
       <c r="C252"/>
       <c r="D252"/>
       <c r="E252" t="s">
-        <v>600</v>
+        <v>2387</v>
       </c>
       <c r="F252" t="s">
         <v>603</v>

</xml_diff>